<commit_message>
added quick bar, expanding grid
</commit_message>
<xml_diff>
--- a/public/shared/excel/anexcel.xlsx
+++ b/public/shared/excel/anexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xForAll\53_AWSSpace\reacthowto\public\shared\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462EC824-D6A1-41E7-B0C2-7151F6190443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3648FF58-700E-484B-BFA3-40FE0562C8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2680" yWindow="630" windowWidth="16510" windowHeight="13240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
-    <t>some value</t>
+    <t>some text from Excel</t>
   </si>
   <si>
-    <t>some text</t>
+    <t>some value from Excel</t>
   </si>
 </sst>
 </file>
@@ -362,18 +362,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>